<commit_message>
Doc fix by konghao
</commit_message>
<xml_diff>
--- a/doc/CallLog.xlsx
+++ b/doc/CallLog.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\UIcase\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9900"/>
   </bookViews>
@@ -41,8 +46,8 @@
   <calcPr calcId="145621" iterateDelta="1E-4"/>
   <customWorkbookViews>
     <customWorkbookView name="konghao - 个人视图" guid="{382531C8-5742-4D50-8FF3-ECE3CBD957B3}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1456" windowHeight="876" activeSheetId="1"/>
+    <customWorkbookView name="Fan xiaohua - 个人视图" guid="{8FE0F79A-9F01-44A1-9BEC-698A5374584F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="563" activeSheetId="1"/>
     <customWorkbookView name="sanyang - 个人视图" guid="{43AE01F4-3A8E-4D81-BC87-E0A8E96B9589}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1596" windowHeight="577" activeSheetId="1"/>
-    <customWorkbookView name="Fan xiaohua - 个人视图" guid="{8FE0F79A-9F01-44A1-9BEC-698A5374584F}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1362" windowHeight="563" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -53,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="123">
   <si>
     <t>编号</t>
   </si>
@@ -3352,10 +3357,6 @@
     <t>【创达】修改序列号，改成171</t>
   </si>
   <si>
-    <t>【创达】为了共享预制数据，前提条件不止存在2条sim卡上的记录</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">前提：手机中有1条SIM1的通话记录，1条SIM2的通话记录
 </t>
@@ -3486,6 +3487,38 @@
   <si>
     <t>【创达】无"查看全部通话记录“button，仅检查进入通话记录界面后有“通话记录”出现,所以拿掉。</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[创达]前提：手机中有已存的通话记录，其中包含已接电话3条、未接电话3条、已拨电话3条
+1.选中全部通话条目
+Assert1：页面上有9条通话记录</t>
+  </si>
+  <si>
+    <t>[创达]前提：手机中有已存的通话记录，其中包含已接电话3条、未接电话3条、已拨电话3条
+1.选中未接电话条目
+Assert1：页面上有3条未接电话通话记录</t>
+  </si>
+  <si>
+    <t>[创达]前提：手机中有已存的通话记录，其中包含已接电话3条、未接电话3条、已拨电话3条
+1.选中已拨电话电话条目
+Assert1：页面上有3条已拨电话通话记录</t>
+  </si>
+  <si>
+    <t>[创达]前提：手机中有已存的通话记录，其中包含已接电话3条、未接电话3条、已拨电话3条
+1.选中已接电话电话条目
+Assert1：页面上有3条已接电话通话记录</t>
+  </si>
+  <si>
+    <t>[创达]前提：手机中有已存的通话记录，3条今天（手机时间上是今天）的通话记录</t>
+  </si>
+  <si>
+    <t>[创达]前提：手机中有已存的通话记录，3条昨天（手机时间上今天，相较于昨天是今天）的通话记录</t>
+  </si>
+  <si>
+    <t>[创达]前提：手机中有已存的通话记录，早于昨天的3条记录（手机时间上是今天，只要比当前时间早二天以上即可）的通话记录</t>
+  </si>
+  <si>
+    <t>【创达】为了共享预制数据，前提条件不止存在2条sim卡上的记录</t>
   </si>
 </sst>
 </file>
@@ -3705,7 +3738,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3813,6 +3846,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -3831,7 +3867,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A4D3CCA2-B664-4F6F-9F5C-FA788A0D3A53}" diskRevisions="1" revisionId="108" version="16">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{B9FA5963-D502-42BC-9A55-70BE8DBE9FD9}" diskRevisions="1" revisionId="126" version="17">
   <header guid="{652CD3C7-F3EE-4642-9B4C-42970E191470}" dateTime="2016-02-25T13:41:43" maxSheetId="2" userName="Fan xiaohua" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
@@ -3912,6 +3948,11 @@
       <sheetId val="1"/>
     </sheetIdMap>
   </header>
+  <header guid="{B9FA5963-D502-42BC-9A55-70BE8DBE9FD9}" dateTime="2016-03-16T09:54:51" maxSheetId="2" userName="konghao" r:id="rId17" minRId="109" maxRId="125">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -4501,6 +4542,439 @@
       </is>
     </nc>
   </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="109" sId="1" xfDxf="1" dxf="1">
+    <nc r="D12" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，其中包含已接电话3条、未接电话3条、已拨电话3条
+1.选中全部通话条目
+Assert1：页面上有9条通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="110" sId="1" xfDxf="1" dxf="1">
+    <nc r="D13" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，其中包含已接电话3条、未接电话3条、已拨电话3条
+1.选中未接电话条目
+Assert1：页面上有3条未接电话通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="111" sId="1" xfDxf="1" dxf="1">
+    <nc r="D14" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，其中包含已接电话3条、未接电话3条、已拨电话3条
+1.选中已拨电话电话条目
+Assert1：页面上有3条已拨电话通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="112" sId="1" xfDxf="1" dxf="1">
+    <nc r="D15" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，其中包含已接电话3条、未接电话3条、已拨电话3条
+1.选中已接电话电话条目
+Assert1：页面上有3条已接电话通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="113" sId="1" xfDxf="1" dxf="1">
+    <nc r="D16" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，3条今天（手机时间上是今天）的通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="114" sId="1" xfDxf="1" dxf="1">
+    <nc r="D17" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，3条昨天（手机时间上今天，相较于昨天是今天）的通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="115" sId="1" xfDxf="1" dxf="1">
+    <nc r="D18" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，早于昨天的3条记录（手机时间上是今天，只要比当前时间早二天以上即可）的通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="116" sId="1" xfDxf="1" dxf="1">
+    <nc r="D19" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，3条今天（手机时间上是今天）的通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="117" sId="1" xfDxf="1" dxf="1">
+    <nc r="D20" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，早于昨天的3条记录（手机时间上是今天，只要比当前时间早二天以上即可）的通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="118" sId="1" xfDxf="1" dxf="1">
+    <nc r="D21" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，早于昨天的3条记录（手机时间上是今天，只要比当前时间早二天以上即可）的通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="119" sId="1" xfDxf="1" dxf="1">
+    <nc r="D22" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，3条今天（手机时间上是今天）的通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="120" sId="1" xfDxf="1" dxf="1">
+    <nc r="D23" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，早于昨天的3条记录（手机时间上是今天，只要比当前时间早二天以上即可）的通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="121" sId="1" xfDxf="1" dxf="1">
+    <nc r="D24" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，早于昨天的3条记录（手机时间上是今天，只要比当前时间早二天以上即可）的通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="122" sId="1" xfDxf="1" dxf="1">
+    <nc r="D25" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，3条今天（手机时间上是今天）的通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="123" sId="1" xfDxf="1" dxf="1">
+    <nc r="D26" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，早于昨天的3条记录（手机时间上是今天，只要比当前时间早二天以上即可）的通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="124" sId="1" xfDxf="1" dxf="1">
+    <nc r="D27" t="inlineStr">
+      <is>
+        <t>[创达]前提：手机中有已存的通话记录，早于昨天的3条记录（手机时间上是今天，只要比当前时间早二天以上即可）的通话记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcc rId="125" sId="1" xfDxf="1" dxf="1">
+    <oc r="D28" t="inlineStr">
+      <is>
+        <t>【创达】为了共享预制数据，前提条件不止存在2条sim卡上的记录</t>
+        <phoneticPr fontId="0" type="noConversion"/>
+      </is>
+    </oc>
+    <nc r="D28" t="inlineStr">
+      <is>
+        <t>【创达】为了共享预制数据，前提条件不止存在2条sim卡上的记录</t>
+      </is>
+    </nc>
+    <ndxf>
+      <alignment vertical="top" wrapText="1" readingOrder="0"/>
+      <border outline="0">
+        <left style="hair">
+          <color auto="1"/>
+        </left>
+        <right style="hair">
+          <color auto="1"/>
+        </right>
+        <top style="hair">
+          <color auto="1"/>
+        </top>
+        <bottom style="hair">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </ndxf>
+  </rcc>
+  <rcv guid="{382531C8-5742-4D50-8FF3-ECE3CBD957B3}" action="delete"/>
+  <rdn rId="0" localSheetId="1" customView="1" name="Z_382531C8_5742_4D50_8FF3_ECE3CBD957B3_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>通话记录!$A$2:$F$72</formula>
+    <oldFormula>通话记录!$A$2:$F$72</oldFormula>
+  </rdn>
+  <rcv guid="{382531C8-5742-4D50-8FF3-ECE3CBD957B3}" action="add"/>
 </revisions>
 </file>
 
@@ -6286,7 +6760,7 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/userNames1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
 <users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
   <userInfo guid="{5CB4F2FF-E7B0-4BF2-A9C7-BF31BBA8C3C1}" name="Fan xiaohua" id="-1996710381" dateTime="2016-03-02T09:45:07"/>
 </users>
@@ -6547,7 +7021,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6557,8 +7031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMA138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -6780,7 +7254,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="11" customFormat="1" ht="64.5" customHeight="1">
+    <row r="12" spans="1:8" s="11" customFormat="1" ht="71.25" customHeight="1">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -6790,7 +7264,9 @@
       <c r="C12" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D12" s="8"/>
+      <c r="D12" s="38" t="s">
+        <v>115</v>
+      </c>
       <c r="E12" s="9" t="s">
         <v>8</v>
       </c>
@@ -6809,7 +7285,9 @@
       <c r="C13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="38" t="s">
+        <v>116</v>
+      </c>
       <c r="E13" s="9" t="s">
         <v>8</v>
       </c>
@@ -6828,7 +7306,9 @@
       <c r="C14" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="38" t="s">
+        <v>117</v>
+      </c>
       <c r="E14" s="9" t="s">
         <v>8</v>
       </c>
@@ -6847,7 +7327,9 @@
       <c r="C15" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="8"/>
+      <c r="D15" s="38" t="s">
+        <v>118</v>
+      </c>
       <c r="E15" s="9" t="s">
         <v>8</v>
       </c>
@@ -6866,7 +7348,9 @@
       <c r="C16" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="8"/>
+      <c r="D16" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="E16" s="9" t="s">
         <v>8</v>
       </c>
@@ -6885,7 +7369,9 @@
       <c r="C17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="8"/>
+      <c r="D17" s="38" t="s">
+        <v>120</v>
+      </c>
       <c r="E17" s="9" t="s">
         <v>8</v>
       </c>
@@ -6904,7 +7390,9 @@
       <c r="C18" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="8"/>
+      <c r="D18" s="38" t="s">
+        <v>121</v>
+      </c>
       <c r="E18" s="9" t="s">
         <v>8</v>
       </c>
@@ -6923,7 +7411,9 @@
       <c r="C19" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="E19" s="9" t="s">
         <v>8</v>
       </c>
@@ -6942,7 +7432,9 @@
       <c r="C20" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="8"/>
+      <c r="D20" s="38" t="s">
+        <v>121</v>
+      </c>
       <c r="E20" s="9" t="s">
         <v>8</v>
       </c>
@@ -6961,7 +7453,9 @@
       <c r="C21" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D21" s="8"/>
+      <c r="D21" s="38" t="s">
+        <v>121</v>
+      </c>
       <c r="E21" s="9" t="s">
         <v>8</v>
       </c>
@@ -6980,7 +7474,9 @@
       <c r="C22" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="8"/>
+      <c r="D22" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="E22" s="9" t="s">
         <v>8</v>
       </c>
@@ -6999,7 +7495,9 @@
       <c r="C23" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="8"/>
+      <c r="D23" s="38" t="s">
+        <v>121</v>
+      </c>
       <c r="E23" s="9" t="s">
         <v>8</v>
       </c>
@@ -7018,7 +7516,9 @@
       <c r="C24" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="8"/>
+      <c r="D24" s="38" t="s">
+        <v>121</v>
+      </c>
       <c r="E24" s="9" t="s">
         <v>8</v>
       </c>
@@ -7037,7 +7537,9 @@
       <c r="C25" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="8"/>
+      <c r="D25" s="38" t="s">
+        <v>119</v>
+      </c>
       <c r="E25" s="9" t="s">
         <v>8</v>
       </c>
@@ -7056,7 +7558,9 @@
       <c r="C26" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="8"/>
+      <c r="D26" s="38" t="s">
+        <v>121</v>
+      </c>
       <c r="E26" s="9" t="s">
         <v>8</v>
       </c>
@@ -7075,7 +7579,9 @@
       <c r="C27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="8"/>
+      <c r="D27" s="38" t="s">
+        <v>121</v>
+      </c>
       <c r="E27" s="9" t="s">
         <v>8</v>
       </c>
@@ -7094,8 +7600,8 @@
       <c r="C28" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>109</v>
+      <c r="D28" s="38" t="s">
+        <v>122</v>
       </c>
       <c r="E28" s="9" t="s">
         <v>8</v>
@@ -7113,7 +7619,7 @@
         <v>36</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D29" s="8"/>
       <c r="E29" s="9" t="s">
@@ -7303,7 +7809,7 @@
         <v>55</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="9" t="s">
@@ -7459,7 +7965,7 @@
         <v>56</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="9" t="s">
@@ -7478,7 +7984,7 @@
         <v>56</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D48" s="8"/>
       <c r="E48" s="9"/>
@@ -7517,7 +8023,7 @@
         <v>65</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E50" s="9" t="s">
         <v>8</v>
@@ -7538,7 +8044,7 @@
         <v>102</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E51" s="9" t="s">
         <v>8</v>
@@ -8299,18 +8805,18 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{382531C8-5742-4D50-8FF3-ECE3CBD957B3}" scale="90" topLeftCell="A10">
-      <selection activeCell="C11" sqref="C11"/>
+    <customSheetView guid="{382531C8-5742-4D50-8FF3-ECE3CBD957B3}" scale="90" topLeftCell="A28">
+      <selection activeCell="D12" sqref="D12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{43AE01F4-3A8E-4D81-BC87-E0A8E96B9589}" scale="90" topLeftCell="A9">
-      <selection activeCell="F74" sqref="F74"/>
+    <customSheetView guid="{8FE0F79A-9F01-44A1-9BEC-698A5374584F}" scale="90">
+      <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId2"/>
     </customSheetView>
-    <customSheetView guid="{8FE0F79A-9F01-44A1-9BEC-698A5374584F}" scale="90">
-      <selection activeCell="B4" sqref="B4"/>
+    <customSheetView guid="{43AE01F4-3A8E-4D81-BC87-E0A8E96B9589}" scale="90" topLeftCell="A9">
+      <selection activeCell="F74" sqref="F74"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
       <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId3"/>
     </customSheetView>

</xml_diff>